<commit_message>
add Sphinx doc for better understanding of code structure by others project's managers and interpreter restructuring
</commit_message>
<xml_diff>
--- a/dataset/models/output/Common-Finance.xlsx
+++ b/dataset/models/output/Common-Finance.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="29">
   <si>
     <t>Common – Financial Environnement</t>
   </si>
@@ -98,7 +98,7 @@
     <t>FOR:INDEX</t>
   </si>
   <si>
-    <t>FOR:DATEPOINT</t>
+    <t>FOR:YEAR</t>
   </si>
   <si>
     <t>FOR:[Market.Nominal WACC]</t>
@@ -117,9 +117,6 @@
   </si>
   <si>
     <t>FOR:[System.Unskilled Labor|Environment]</t>
-  </si>
-  <si>
-    <t/>
   </si>
 </sst>
 </file>
@@ -129,7 +126,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="#,##0.00%"/>
   </numFmts>
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -146,7 +143,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -163,12 +160,6 @@
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
       <family val="2"/>
     </font>
     <font>
@@ -269,7 +260,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="22">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
@@ -289,11 +280,11 @@
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="5" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="6" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="5" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="7" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -301,37 +292,31 @@
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="8" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="9" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="5" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="6" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="10" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="10" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="4" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="7" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="11" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="11" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="5" applyFont="1" fillId="4" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="5" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="5" applyFont="1" fillId="0" quotePrefix="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="8" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="5" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
@@ -648,32 +633,32 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="22" width="2.7192857142857143" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="22" width="1.5764285714285713" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="22" width="2.7192857142857143" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="22" width="12.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="22" width="21.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="22" width="20.862142857142857" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="22" width="9.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="22" width="16.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="9" max="9" style="23" width="9.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="10" max="10" style="22" width="14.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="11" max="11" style="22" width="6.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="12" max="12" style="22" width="23.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="13" max="13" style="22" width="7.147857142857143" customWidth="1" bestFit="1"/>
-    <col min="14" max="14" style="22" width="23.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="15" max="15" style="22" width="6.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="16" max="16" style="22" width="23.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="17" max="17" style="22" width="6.576428571428571" customWidth="1" bestFit="1"/>
-    <col min="18" max="18" style="22" width="9.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="19" max="19" style="22" width="6.147857142857143" customWidth="1" bestFit="1"/>
-    <col min="20" max="20" style="22" width="8.005" customWidth="1" bestFit="1"/>
-    <col min="21" max="21" style="22" width="7.2907142857142855" customWidth="1" bestFit="1"/>
-    <col min="22" max="22" style="22" width="5.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="23" max="23" style="22" width="8.005" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="20" width="2.7192857142857143" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="20" width="1.5764285714285713" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="20" width="2.7192857142857143" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="20" width="12.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="20" width="21.290714285714284" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="20" width="20.862142857142857" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="20" width="9.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="20" width="16.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="9" max="9" style="21" width="9.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="10" max="10" style="20" width="14.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="11" max="11" style="20" width="6.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="12" max="12" style="20" width="23.290714285714284" customWidth="1" bestFit="1"/>
+    <col min="13" max="13" style="20" width="7.147857142857143" customWidth="1" bestFit="1"/>
+    <col min="14" max="14" style="20" width="23.290714285714284" customWidth="1" bestFit="1"/>
+    <col min="15" max="15" style="20" width="6.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="16" max="16" style="20" width="23.290714285714284" customWidth="1" bestFit="1"/>
+    <col min="17" max="17" style="20" width="6.576428571428571" customWidth="1" bestFit="1"/>
+    <col min="18" max="18" style="20" width="9.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="19" max="19" style="20" width="6.147857142857143" customWidth="1" bestFit="1"/>
+    <col min="20" max="20" style="20" width="8.005" customWidth="1" bestFit="1"/>
+    <col min="21" max="21" style="20" width="7.2907142857142855" customWidth="1" bestFit="1"/>
+    <col min="22" max="22" style="20" width="5.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="23" max="23" style="20" width="8.005" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="24">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="24.75">
       <c r="A1" s="1"/>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -719,7 +704,7 @@
       <c r="N2" s="1"/>
       <c r="O2" s="1"/>
       <c r="P2" s="1"/>
-      <c r="Q2" s="6"/>
+      <c r="Q2" s="3"/>
       <c r="R2" s="1"/>
       <c r="S2" s="1"/>
       <c r="T2" s="1"/>
@@ -729,20 +714,20 @@
     </row>
     <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
       <c r="A3" s="1"/>
-      <c r="B3" s="7"/>
+      <c r="B3" s="6"/>
       <c r="C3" s="1"/>
-      <c r="D3" s="6" t="s">
+      <c r="D3" s="3" t="s">
         <v>2</v>
       </c>
       <c r="E3" s="1"/>
-      <c r="F3" s="8" t="s">
+      <c r="F3" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="G3" s="6" t="s">
+      <c r="G3" s="3" t="s">
         <v>4</v>
       </c>
       <c r="H3" s="1"/>
-      <c r="I3" s="9"/>
+      <c r="I3" s="8"/>
       <c r="J3" s="1"/>
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
@@ -761,15 +746,15 @@
     <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
-      <c r="C4" s="10"/>
-      <c r="D4" s="6" t="s">
+      <c r="C4" s="9"/>
+      <c r="D4" s="3" t="s">
         <v>5</v>
       </c>
       <c r="E4" s="1"/>
-      <c r="F4" s="8" t="s">
+      <c r="F4" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="G4" s="6" t="s">
+      <c r="G4" s="3" t="s">
         <v>4</v>
       </c>
       <c r="H4" s="1"/>
@@ -781,7 +766,7 @@
       <c r="N4" s="1"/>
       <c r="O4" s="1"/>
       <c r="P4" s="1"/>
-      <c r="Q4" s="11" t="s">
+      <c r="Q4" s="10" t="s">
         <v>7</v>
       </c>
       <c r="R4" s="1"/>
@@ -795,14 +780,14 @@
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
-      <c r="D5" s="6" t="s">
+      <c r="D5" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E5" s="1"/>
-      <c r="F5" s="12" t="s">
+      <c r="F5" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="G5" s="6" t="s">
+      <c r="G5" s="3" t="s">
         <v>10</v>
       </c>
       <c r="H5" s="1"/>
@@ -828,10 +813,10 @@
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
-      <c r="F6" s="12" t="s">
+      <c r="F6" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="G6" s="6" t="s">
+      <c r="G6" s="3" t="s">
         <v>12</v>
       </c>
       <c r="H6" s="1"/>
@@ -853,21 +838,21 @@
     </row>
     <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
       <c r="A7" s="1"/>
-      <c r="B7" s="9"/>
-      <c r="C7" s="13"/>
-      <c r="D7" s="7"/>
+      <c r="B7" s="8"/>
+      <c r="C7" s="12"/>
+      <c r="D7" s="6"/>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
       <c r="I7" s="3"/>
-      <c r="J7" s="14"/>
-      <c r="K7" s="9"/>
-      <c r="L7" s="14"/>
-      <c r="M7" s="9"/>
-      <c r="N7" s="14"/>
+      <c r="J7" s="13"/>
+      <c r="K7" s="8"/>
+      <c r="L7" s="13"/>
+      <c r="M7" s="8"/>
+      <c r="N7" s="13"/>
       <c r="O7" s="1"/>
-      <c r="P7" s="14"/>
+      <c r="P7" s="13"/>
       <c r="Q7" s="1"/>
       <c r="R7" s="1"/>
       <c r="S7" s="1"/>
@@ -880,33 +865,33 @@
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
-      <c r="D8" s="15" t="s">
+      <c r="D8" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="E8" s="15" t="s">
+      <c r="E8" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="F8" s="15" t="s">
+      <c r="F8" s="14" t="s">
         <v>15</v>
       </c>
       <c r="G8" s="1"/>
-      <c r="H8" s="15" t="s">
+      <c r="H8" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="I8" s="16"/>
-      <c r="J8" s="15" t="s">
+      <c r="I8" s="15"/>
+      <c r="J8" s="14" t="s">
         <v>17</v>
       </c>
       <c r="K8" s="1"/>
-      <c r="L8" s="15" t="s">
+      <c r="L8" s="14" t="s">
         <v>18</v>
       </c>
       <c r="M8" s="1"/>
-      <c r="N8" s="15" t="s">
+      <c r="N8" s="14" t="s">
         <v>19</v>
       </c>
       <c r="O8" s="1"/>
-      <c r="P8" s="15" t="s">
+      <c r="P8" s="14" t="s">
         <v>20</v>
       </c>
       <c r="Q8" s="1"/>
@@ -921,39 +906,37 @@
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
-      <c r="D9" s="17" t="s">
+      <c r="D9" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="E9" s="17" t="s">
+      <c r="E9" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="F9" s="8" t="s">
+      <c r="F9" s="7" t="s">
         <v>23</v>
       </c>
       <c r="G9" s="1"/>
-      <c r="H9" s="8" t="s">
+      <c r="H9" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="I9" s="18"/>
-      <c r="J9" s="12" t="s">
+      <c r="I9" s="17"/>
+      <c r="J9" s="11" t="s">
         <v>25</v>
       </c>
       <c r="K9" s="1"/>
-      <c r="L9" s="8" t="s">
+      <c r="L9" s="7" t="s">
         <v>26</v>
       </c>
       <c r="M9" s="1"/>
-      <c r="N9" s="8" t="s">
+      <c r="N9" s="7" t="s">
         <v>27</v>
       </c>
       <c r="O9" s="1"/>
-      <c r="P9" s="8" t="s">
+      <c r="P9" s="7" t="s">
         <v>28</v>
       </c>
       <c r="Q9" s="1"/>
-      <c r="R9" s="19" t="s">
-        <v>29</v>
-      </c>
+      <c r="R9" s="17"/>
       <c r="S9" s="1"/>
       <c r="T9" s="1"/>
       <c r="U9" s="1"/>
@@ -961,7 +944,7 @@
       <c r="W9" s="1"/>
     </row>
     <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="19.5">
-      <c r="A10" s="13"/>
+      <c r="A10" s="12"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
@@ -976,19 +959,17 @@
       <c r="M10" s="1"/>
       <c r="N10" s="1"/>
       <c r="O10" s="1"/>
-      <c r="P10" s="20"/>
-      <c r="Q10" s="13"/>
-      <c r="R10" s="19" t="s">
-        <v>29</v>
-      </c>
-      <c r="S10" s="13"/>
-      <c r="T10" s="13"/>
-      <c r="U10" s="13"/>
-      <c r="V10" s="13"/>
-      <c r="W10" s="13"/>
+      <c r="P10" s="18"/>
+      <c r="Q10" s="12"/>
+      <c r="R10" s="17"/>
+      <c r="S10" s="12"/>
+      <c r="T10" s="12"/>
+      <c r="U10" s="12"/>
+      <c r="V10" s="12"/>
+      <c r="W10" s="12"/>
     </row>
     <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="19.5">
-      <c r="A11" s="13"/>
+      <c r="A11" s="12"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
@@ -1003,14 +984,14 @@
       <c r="M11" s="1"/>
       <c r="N11" s="1"/>
       <c r="O11" s="1"/>
-      <c r="P11" s="20"/>
-      <c r="Q11" s="13"/>
-      <c r="R11" s="21"/>
-      <c r="S11" s="13"/>
-      <c r="T11" s="13"/>
-      <c r="U11" s="13"/>
-      <c r="V11" s="13"/>
-      <c r="W11" s="13"/>
+      <c r="P11" s="18"/>
+      <c r="Q11" s="12"/>
+      <c r="R11" s="19"/>
+      <c r="S11" s="12"/>
+      <c r="T11" s="12"/>
+      <c r="U11" s="12"/>
+      <c r="V11" s="12"/>
+      <c r="W11" s="12"/>
     </row>
     <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18.75">
       <c r="A12" s="1"/>
@@ -1030,7 +1011,7 @@
       <c r="O12" s="1"/>
       <c r="P12" s="1"/>
       <c r="Q12" s="1"/>
-      <c r="R12" s="21"/>
+      <c r="R12" s="19"/>
       <c r="S12" s="1"/>
       <c r="T12" s="1"/>
       <c r="U12" s="1"/>
@@ -1055,7 +1036,7 @@
       <c r="O13" s="1"/>
       <c r="P13" s="1"/>
       <c r="Q13" s="1"/>
-      <c r="R13" s="21"/>
+      <c r="R13" s="19"/>
       <c r="S13" s="1"/>
       <c r="T13" s="1"/>
       <c r="U13" s="1"/>
@@ -1080,7 +1061,7 @@
       <c r="O14" s="1"/>
       <c r="P14" s="1"/>
       <c r="Q14" s="1"/>
-      <c r="R14" s="21"/>
+      <c r="R14" s="19"/>
       <c r="S14" s="1"/>
       <c r="T14" s="1"/>
       <c r="U14" s="1"/>
@@ -1105,7 +1086,7 @@
       <c r="O15" s="1"/>
       <c r="P15" s="1"/>
       <c r="Q15" s="1"/>
-      <c r="R15" s="21"/>
+      <c r="R15" s="19"/>
       <c r="S15" s="1"/>
       <c r="T15" s="1"/>
       <c r="U15" s="1"/>
@@ -1130,7 +1111,7 @@
       <c r="O16" s="1"/>
       <c r="P16" s="1"/>
       <c r="Q16" s="1"/>
-      <c r="R16" s="21"/>
+      <c r="R16" s="19"/>
       <c r="S16" s="1"/>
       <c r="T16" s="1"/>
       <c r="U16" s="1"/>
@@ -1155,7 +1136,7 @@
       <c r="O17" s="1"/>
       <c r="P17" s="1"/>
       <c r="Q17" s="1"/>
-      <c r="R17" s="21"/>
+      <c r="R17" s="19"/>
       <c r="S17" s="1"/>
       <c r="T17" s="1"/>
       <c r="U17" s="1"/>
@@ -1180,7 +1161,7 @@
       <c r="O18" s="1"/>
       <c r="P18" s="1"/>
       <c r="Q18" s="1"/>
-      <c r="R18" s="21"/>
+      <c r="R18" s="19"/>
       <c r="S18" s="1"/>
       <c r="T18" s="1"/>
       <c r="U18" s="1"/>
@@ -1205,7 +1186,7 @@
       <c r="O19" s="1"/>
       <c r="P19" s="1"/>
       <c r="Q19" s="1"/>
-      <c r="R19" s="21"/>
+      <c r="R19" s="19"/>
       <c r="S19" s="1"/>
       <c r="T19" s="1"/>
       <c r="U19" s="1"/>
@@ -1230,7 +1211,7 @@
       <c r="O20" s="1"/>
       <c r="P20" s="1"/>
       <c r="Q20" s="1"/>
-      <c r="R20" s="21"/>
+      <c r="R20" s="19"/>
       <c r="S20" s="1"/>
       <c r="T20" s="1"/>
       <c r="U20" s="1"/>
@@ -1255,7 +1236,7 @@
       <c r="O21" s="1"/>
       <c r="P21" s="1"/>
       <c r="Q21" s="1"/>
-      <c r="R21" s="21"/>
+      <c r="R21" s="19"/>
       <c r="S21" s="1"/>
       <c r="T21" s="1"/>
       <c r="U21" s="1"/>
@@ -1280,7 +1261,7 @@
       <c r="O22" s="1"/>
       <c r="P22" s="1"/>
       <c r="Q22" s="1"/>
-      <c r="R22" s="21"/>
+      <c r="R22" s="19"/>
       <c r="S22" s="1"/>
       <c r="T22" s="1"/>
       <c r="U22" s="1"/>
@@ -1305,7 +1286,7 @@
       <c r="O23" s="1"/>
       <c r="P23" s="1"/>
       <c r="Q23" s="1"/>
-      <c r="R23" s="21"/>
+      <c r="R23" s="19"/>
       <c r="S23" s="1"/>
       <c r="T23" s="1"/>
       <c r="U23" s="1"/>
@@ -1330,14 +1311,14 @@
       <c r="O24" s="1"/>
       <c r="P24" s="1"/>
       <c r="Q24" s="1"/>
-      <c r="R24" s="21"/>
+      <c r="R24" s="19"/>
       <c r="S24" s="1"/>
       <c r="T24" s="1"/>
       <c r="U24" s="1"/>
       <c r="V24" s="1"/>
       <c r="W24" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="18.75">
       <c r="A25" s="1"/>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
@@ -1355,14 +1336,14 @@
       <c r="O25" s="1"/>
       <c r="P25" s="1"/>
       <c r="Q25" s="1"/>
-      <c r="R25" s="21"/>
+      <c r="R25" s="19"/>
       <c r="S25" s="1"/>
       <c r="T25" s="1"/>
       <c r="U25" s="1"/>
       <c r="V25" s="1"/>
       <c r="W25" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="18.75">
       <c r="A26" s="1"/>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
@@ -1380,14 +1361,14 @@
       <c r="O26" s="1"/>
       <c r="P26" s="1"/>
       <c r="Q26" s="1"/>
-      <c r="R26" s="21"/>
+      <c r="R26" s="19"/>
       <c r="S26" s="1"/>
       <c r="T26" s="1"/>
       <c r="U26" s="1"/>
       <c r="V26" s="1"/>
       <c r="W26" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="18.75">
       <c r="A27" s="1"/>
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
@@ -1405,14 +1386,14 @@
       <c r="O27" s="1"/>
       <c r="P27" s="1"/>
       <c r="Q27" s="1"/>
-      <c r="R27" s="21"/>
+      <c r="R27" s="19"/>
       <c r="S27" s="1"/>
       <c r="T27" s="1"/>
       <c r="U27" s="1"/>
       <c r="V27" s="1"/>
       <c r="W27" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="18.75">
       <c r="A28" s="1"/>
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
@@ -1430,14 +1411,14 @@
       <c r="O28" s="1"/>
       <c r="P28" s="1"/>
       <c r="Q28" s="1"/>
-      <c r="R28" s="21"/>
+      <c r="R28" s="19"/>
       <c r="S28" s="1"/>
       <c r="T28" s="1"/>
       <c r="U28" s="1"/>
       <c r="V28" s="1"/>
       <c r="W28" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="18.75">
       <c r="A29" s="1"/>
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
@@ -1455,14 +1436,14 @@
       <c r="O29" s="1"/>
       <c r="P29" s="1"/>
       <c r="Q29" s="1"/>
-      <c r="R29" s="21"/>
+      <c r="R29" s="19"/>
       <c r="S29" s="1"/>
       <c r="T29" s="1"/>
       <c r="U29" s="1"/>
       <c r="V29" s="1"/>
       <c r="W29" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="18.75">
       <c r="A30" s="1"/>
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
@@ -1480,14 +1461,14 @@
       <c r="O30" s="1"/>
       <c r="P30" s="1"/>
       <c r="Q30" s="1"/>
-      <c r="R30" s="21"/>
+      <c r="R30" s="19"/>
       <c r="S30" s="1"/>
       <c r="T30" s="1"/>
       <c r="U30" s="1"/>
       <c r="V30" s="1"/>
       <c r="W30" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="18.75">
       <c r="A31" s="1"/>
       <c r="B31" s="1"/>
       <c r="C31" s="1"/>
@@ -1505,14 +1486,14 @@
       <c r="O31" s="1"/>
       <c r="P31" s="1"/>
       <c r="Q31" s="1"/>
-      <c r="R31" s="21"/>
+      <c r="R31" s="19"/>
       <c r="S31" s="1"/>
       <c r="T31" s="1"/>
       <c r="U31" s="1"/>
       <c r="V31" s="1"/>
       <c r="W31" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="18.75">
       <c r="A32" s="1"/>
       <c r="B32" s="1"/>
       <c r="C32" s="1"/>
@@ -1530,7 +1511,7 @@
       <c r="O32" s="1"/>
       <c r="P32" s="1"/>
       <c r="Q32" s="1"/>
-      <c r="R32" s="21"/>
+      <c r="R32" s="19"/>
       <c r="S32" s="1"/>
       <c r="T32" s="1"/>
       <c r="U32" s="1"/>
@@ -1555,7 +1536,7 @@
       <c r="O33" s="1"/>
       <c r="P33" s="1"/>
       <c r="Q33" s="1"/>
-      <c r="R33" s="21"/>
+      <c r="R33" s="19"/>
       <c r="S33" s="1"/>
       <c r="T33" s="1"/>
       <c r="U33" s="1"/>
@@ -1580,7 +1561,7 @@
       <c r="O34" s="1"/>
       <c r="P34" s="1"/>
       <c r="Q34" s="1"/>
-      <c r="R34" s="21"/>
+      <c r="R34" s="19"/>
       <c r="S34" s="1"/>
       <c r="T34" s="1"/>
       <c r="U34" s="1"/>
@@ -1605,7 +1586,7 @@
       <c r="O35" s="1"/>
       <c r="P35" s="1"/>
       <c r="Q35" s="1"/>
-      <c r="R35" s="21"/>
+      <c r="R35" s="19"/>
       <c r="S35" s="1"/>
       <c r="T35" s="1"/>
       <c r="U35" s="1"/>
@@ -2171,7 +2152,7 @@
       <c r="F58" s="1"/>
       <c r="G58" s="1"/>
       <c r="H58" s="1"/>
-      <c r="I58" s="13"/>
+      <c r="I58" s="12"/>
       <c r="J58" s="1"/>
       <c r="K58" s="1"/>
       <c r="L58" s="1"/>

</xml_diff>